<commit_message>
rename the files for each group
</commit_message>
<xml_diff>
--- a/xx班xx组/00班00组1stHomework.xlsx
+++ b/xx班xx组/00班00组1stHomework.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jxl\Desktop\高级英语写作\jxl\00班00组\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdvancedWriting2024\AdvancedWriting2024\xx班xx组\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D24C2F9E-33FE-4B2A-A0E2-98B4C49CB89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C63BEB8-62CA-467B-ABA8-716664732708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9AF7645E-0F89-4DFA-8157-AC13E33203E1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AF7645E-0F89-4DFA-8157-AC13E33203E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,122 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>jxl</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{C5266E2A-98B2-498A-80EA-BB96BE912F5F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>jxl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+用阿拉伯数字，提供的组号和提交给班长的组号一致，不确定的同学可以到分组.xlsx文件中查询</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{33734286-5CFD-4288-A664-B98AC269EADA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>jxl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+该学生分析的论文题目，这篇论文需包含在上传的文献里</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{F1F306E3-EFD5-476F-B348-DEE025EA6311}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>jxl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+第一次作业不需要对abstract分析</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{473CF798-094A-4753-A7CC-162B1F7CC08F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>jxl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+对于每一个部分列出outline（subheadings），如果能对每个subheadings的内容用一两句英文总结更佳</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Abstract</t>
   </si>
@@ -92,12 +206,67 @@
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>Objectification strategies outperform subjectification
+strategies in military interventionist discourses</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conclusion</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1 Descriptive statistic and reliabilities
+4.2 Test of Hypothesis</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.1 Participants
+3.2 Materials and design
+3.3 Measures</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>divided into two sections
+1.  Introduction
+2. Background</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>combined with conclusion</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>combined with discussion</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Appendix</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reference</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data Source</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Appendix 1. Experimental stimuli
+Appendix 2. Scales and Manipulation checks</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>provide the source for the news used in this study</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +313,21 @@
       <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -573,23 +757,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A14700-4374-49E4-9B5E-A9D8A3E19867}">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A14700-4374-49E4-9B5E-A9D8A3E19867}">
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="43.1640625" customWidth="1"/>
     <col min="5" max="5" width="21.08203125" customWidth="1"/>
-    <col min="6" max="6" width="16.9140625" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.58203125" customWidth="1"/>
-    <col min="9" max="9" width="15.75" customWidth="1"/>
+    <col min="6" max="6" width="23.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.08203125" customWidth="1"/>
+    <col min="8" max="8" width="33.58203125" customWidth="1"/>
+    <col min="9" max="10" width="15.75" customWidth="1"/>
+    <col min="11" max="11" width="27" customWidth="1"/>
+    <col min="12" max="13" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="47.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -617,23 +804,55 @@
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="95.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
-        <v>2</v>
+    <row r="3" spans="1:13" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -643,10 +862,14 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
-        <v>3</v>
+    <row r="4" spans="1:13" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -656,10 +879,14 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>4</v>
+    <row r="5" spans="1:13" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -669,10 +896,14 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
-        <v>5</v>
+    <row r="6" spans="1:13" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -682,10 +913,14 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
-        <v>6</v>
+    <row r="7" spans="1:13" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -695,10 +930,14 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
-        <v>7</v>
+    <row r="8" spans="1:13" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -708,9 +947,14 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>